<commit_message>
minor fixes in wording and grammar
</commit_message>
<xml_diff>
--- a/admin/temp/seats_data.xlsx
+++ b/admin/temp/seats_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>user_id</t>
   </si>
@@ -25,10 +25,19 @@
     <t>timestamp</t>
   </si>
   <si>
+    <t>admin</t>
+  </si>
+  <si>
     <t>bogdan.yakupov@nu.edu.kz</t>
   </si>
   <si>
-    <t>Main hall_main_0_0</t>
+    <t>Main hall_0_main_3_2</t>
+  </si>
+  <si>
+    <t>Main hall_0_main_3_4</t>
+  </si>
+  <si>
+    <t>Main hall_0_main_0_3</t>
   </si>
 </sst>
 </file>
@@ -390,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -415,10 +424,38 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="2">
+        <v>45500.23421097222</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="2">
-        <v>45494.61670138889</v>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="2">
+        <v>45500.23984773971</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="2">
+        <v>45500.24039318286</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
button 'to join queue' now greys off if the user has already booked a place or joined a queue; added history page with recent bookings; clock counts down until one reaches queue_finish constraint; no icons on pages, like hamburger on the events page (to eliminate possible UX misunderstanding); now queue displays 'missed' if one has missed their queue; now it sends messages on the email containing queue start\end time
</commit_message>
<xml_diff>
--- a/admin/temp/seats_data.xlsx
+++ b/admin/temp/seats_data.xlsx
@@ -14,12 +14,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
   <si>
     <t>user_id</t>
   </si>
   <si>
-    <t>place_id</t>
+    <t>loadable_place_id</t>
   </si>
   <si>
     <t>timestamp</t>
@@ -28,16 +28,13 @@
     <t>admin</t>
   </si>
   <si>
-    <t>bogdan.yakupov@nu.edu.kz</t>
-  </si>
-  <si>
-    <t>Main hall_0_main_3_2</t>
-  </si>
-  <si>
-    <t>Main hall_0_main_3_4</t>
-  </si>
-  <si>
-    <t>Main hall_0_main_0_3</t>
+    <t>Test event 1; Cinema hall, floor 1, upper middle section, row 6, seat 3</t>
+  </si>
+  <si>
+    <t>Test event 1; Cinema hall, floor 1, upper middle section, row 4, seat 2</t>
+  </si>
+  <si>
+    <t>Test event 1; Cinema hall, floor 1, upper middle section, row 8, seat 3</t>
   </si>
 </sst>
 </file>
@@ -424,10 +421,10 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D2" s="2">
-        <v>45500.23421097222</v>
+        <v>45508.49006479167</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -435,13 +432,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D3" s="2">
-        <v>45500.23984773971</v>
+        <v>45508.49010777778</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -452,10 +449,10 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D4" s="2">
-        <v>45500.24039318286</v>
+        <v>45508.49005549768</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed issue with acquiring time from an external API (now it uses server proxy to get an access to worldtimeapi)
</commit_message>
<xml_diff>
--- a/admin/temp/seats_data.xlsx
+++ b/admin/temp/seats_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
   <si>
     <t>user_id</t>
   </si>
@@ -28,22 +28,34 @@
     <t>admin</t>
   </si>
   <si>
+    <t>bogdan@nu.edu.kz</t>
+  </si>
+  <si>
     <t>bogdan.yakupov@nu.edu.kz</t>
   </si>
   <si>
-    <t>Test event 1; Cinema hall, floor 1, upper middle section, row 6, seat 3</t>
-  </si>
-  <si>
-    <t>Test event 1; Cinema hall, floor 1, upper middle section, row 8, seat 3</t>
-  </si>
-  <si>
-    <t>Test event 1; Cinema hall, floor 1, upper left section, row 4, seat 3</t>
-  </si>
-  <si>
-    <t>Test event 1; Cinema hall, floor 1, upper middle section, row 4, seat 2</t>
-  </si>
-  <si>
-    <t>Test event 1; Cinema hall, floor 1, upper left section, row 6, seat 2</t>
+    <t>Cinema hall, floor 1, upper middle section, row D, seat 2</t>
+  </si>
+  <si>
+    <t>Cinema hall, floor 1, upper middle section, row H, seat 3</t>
+  </si>
+  <si>
+    <t>Cinema hall, floor 1, upper left section, row H, seat 3</t>
+  </si>
+  <si>
+    <t>Cinema hall, floor 1, upper left section, row F, seat 2</t>
+  </si>
+  <si>
+    <t>Cinema hall, floor 1, upper middle section, row F, seat 5</t>
+  </si>
+  <si>
+    <t>Cinema hall, floor 1, upper left section, row F, seat 4</t>
+  </si>
+  <si>
+    <t>Cinema hall, floor 1, upper left section, row E, seat 4</t>
+  </si>
+  <si>
+    <t>Cinema hall, floor 1, upper left section, row A, seat 1</t>
   </si>
 </sst>
 </file>
@@ -405,7 +417,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -430,10 +442,10 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D2" s="2">
-        <v>45508.49006479167</v>
+        <v>45508.49010777778</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -444,7 +456,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D3" s="2">
         <v>45508.49005549768</v>
@@ -455,13 +467,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D4" s="2">
-        <v>45509.57801660212</v>
+        <v>45517.61121153936</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -472,10 +484,10 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D5" s="2">
-        <v>45508.49010777778</v>
+        <v>45509.57961226852</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -483,13 +495,55 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D6" s="2">
-        <v>45509.57961226852</v>
+        <v>45509.62525357998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="2">
+        <v>45511.72776239251</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="2">
+        <v>45517.61121153936</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="2">
+        <v>45517.61521243056</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
integrated permission check in tokens; now seats are booked by their letter and seat number
</commit_message>
<xml_diff>
--- a/admin/temp/seats_data.xlsx
+++ b/admin/temp/seats_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>user_id</t>
   </si>
@@ -25,37 +25,31 @@
     <t>timestamp</t>
   </si>
   <si>
+    <t>bogdan@nu.edu.kz</t>
+  </si>
+  <si>
     <t>admin</t>
   </si>
   <si>
-    <t>bogdan@nu.edu.kz</t>
-  </si>
-  <si>
     <t>bogdan.yakupov@nu.edu.kz</t>
   </si>
   <si>
-    <t>Cinema hall, floor 1, upper middle section, row D, seat 2</t>
-  </si>
-  <si>
-    <t>Cinema hall, floor 1, upper middle section, row H, seat 3</t>
-  </si>
-  <si>
-    <t>Cinema hall, floor 1, upper left section, row H, seat 3</t>
-  </si>
-  <si>
-    <t>Cinema hall, floor 1, upper left section, row F, seat 2</t>
-  </si>
-  <si>
-    <t>Cinema hall, floor 1, upper middle section, row F, seat 5</t>
-  </si>
-  <si>
-    <t>Cinema hall, floor 1, upper left section, row F, seat 4</t>
-  </si>
-  <si>
-    <t>Cinema hall, floor 1, upper left section, row E, seat 4</t>
-  </si>
-  <si>
-    <t>Cinema hall, floor 1, upper left section, row A, seat 1</t>
+    <t>adema.akizhanova@nu.edu.kz</t>
+  </si>
+  <si>
+    <t>Test event 1; Cinema hall, floor 1, upper middle section, row F, seat 5</t>
+  </si>
+  <si>
+    <t>Test event 1; Cinema hall, floor 1, upper middle section, row H, seat 3</t>
+  </si>
+  <si>
+    <t>Test event 1; Cinema hall, floor 1, upper middle section, row D, seat 2</t>
+  </si>
+  <si>
+    <t>Test event 1; Cinema hall, floor 1, upper left section, row F, seat 3</t>
+  </si>
+  <si>
+    <t>Test event 1; Cinema hall, floor 1, upper left section, row G, seat 6</t>
   </si>
 </sst>
 </file>
@@ -417,7 +411,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -442,10 +436,10 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2" s="2">
-        <v>45508.49010777778</v>
+        <v>45509.62525357998</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -453,10 +447,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D3" s="2">
         <v>45508.49005549768</v>
@@ -467,13 +461,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D4" s="2">
-        <v>45517.61121153936</v>
+        <v>45508.49010777778</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -481,13 +475,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D5" s="2">
-        <v>45509.57961226852</v>
+        <v>45519.62325730543</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -495,55 +489,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D6" s="2">
-        <v>45509.62525357998</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="1">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="2">
-        <v>45511.72776239251</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="1">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="2">
-        <v>45517.61121153936</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="1">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="2">
-        <v>45517.61521243056</v>
+        <v>45519.62876581898</v>
       </c>
     </row>
   </sheetData>

</xml_diff>